<commit_message>
fix the multigrid styling issues
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>commit code</t>
+  </si>
+  <si>
+    <t>use multi grid with fixed employee id column to display the data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix the styling issues </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing the screen </t>
   </si>
 </sst>
 </file>
@@ -409,16 +418,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -594,10 +604,49 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>45214</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45214</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45214</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45240</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing Employee Import Completed
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -100,6 +101,36 @@
   </si>
   <si>
     <t xml:space="preserve">testing the screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Employee Screen Client side </t>
+  </si>
+  <si>
+    <t>Create Employee Screen Validations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Employee Screen Servier side </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify Employee </t>
+  </si>
+  <si>
+    <t>Navigation from List to Create screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demo the screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">split the utility into a separate application </t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>no error thrown but said import success</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -418,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +679,88 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
+      <c r="B20" s="1">
+        <v>45248</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create Employee Screen Integration Basic
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5595"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="Test data backup" sheetId="4" r:id="rId3"/>
+    <sheet name="create employee screen" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -131,13 +133,142 @@
   </si>
   <si>
     <t>fixed</t>
+  </si>
+  <si>
+    <t>Sl.No</t>
+  </si>
+  <si>
+    <t>Employee code</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>Name of father / husband</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Date of joining</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>IFSC Code</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>Pan Number</t>
+  </si>
+  <si>
+    <t>Aadhar Number</t>
+  </si>
+  <si>
+    <t>UAN EPF</t>
+  </si>
+  <si>
+    <t>EPF No</t>
+  </si>
+  <si>
+    <t>ESI Number</t>
+  </si>
+  <si>
+    <t>Welfare Fund Number</t>
+  </si>
+  <si>
+    <t>EPF Nominee</t>
+  </si>
+  <si>
+    <t>EPF Nominee Relation</t>
+  </si>
+  <si>
+    <t>ESI Nominee</t>
+  </si>
+  <si>
+    <t>ESI Nominee Relation</t>
+  </si>
+  <si>
+    <t>GPAIP Nominee</t>
+  </si>
+  <si>
+    <t>GPAIP Nominee Relation</t>
+  </si>
+  <si>
+    <t>Gratuity Nominee</t>
+  </si>
+  <si>
+    <t>Gratuity Nominee Relation</t>
+  </si>
+  <si>
+    <t>Last Working Date</t>
+  </si>
+  <si>
+    <t>Date of Releaving</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Contact Information</t>
+  </si>
+  <si>
+    <t>Employment Information</t>
+  </si>
+  <si>
+    <t>Personal Information</t>
+  </si>
+  <si>
+    <t>Bank Information</t>
+  </si>
+  <si>
+    <t>Identity Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nominees </t>
+  </si>
+  <si>
+    <t>A-300</t>
+  </si>
+  <si>
+    <t>Anish</t>
+  </si>
+  <si>
+    <t>Anish Bhavan</t>
+  </si>
+  <si>
+    <t>in save api the req.body is printing an empty obj</t>
+  </si>
+  <si>
+    <t>open bugs = fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,16 +276,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="A\ham"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,13 +312,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,18 +639,17 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -477,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -488,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -499,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -510,7 +696,7 @@
         <v>45193</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -521,7 +707,7 @@
         <v>45193</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -532,7 +718,7 @@
         <v>45193</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -543,7 +729,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -551,7 +737,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -559,7 +745,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -570,7 +756,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -581,7 +767,7 @@
         <v>45201</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -592,7 +778,7 @@
         <v>45206</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -603,7 +789,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -617,7 +803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -631,7 +817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -642,7 +828,7 @@
         <v>45214</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -653,7 +839,7 @@
         <v>45214</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -664,7 +850,7 @@
         <v>45224</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -675,7 +861,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -686,47 +872,62 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>45276</v>
+      </c>
+      <c r="C22" s="9">
+        <v>45276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
+        <v>45276</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45277</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -738,28 +939,234 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>9447757072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="24">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="36">
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="36">
+      <c r="K7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="36">
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="36">
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="36">
+      <c r="B16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="36">
+      <c r="B18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="36">
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="36">
+      <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Employee Screen Validations
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -639,7 +639,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -905,6 +905,12 @@
     <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>28</v>
+      </c>
+      <c r="B24" s="9">
+        <v>45277</v>
+      </c>
+      <c r="C24" s="9">
+        <v>45277</v>
       </c>
     </row>
     <row r="25" spans="1:4">

</xml_diff>

<commit_message>
Move loader into a separate application
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -937,11 +937,23 @@
       <c r="A26" t="s">
         <v>31</v>
       </c>
+      <c r="B26" s="9">
+        <v>45287</v>
+      </c>
+      <c r="C26" s="9">
+        <v>45287</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>26</v>
       </c>
+      <c r="B27" s="9">
+        <v>45287</v>
+      </c>
+      <c r="C27" s="9">
+        <v>45287</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
@@ -951,6 +963,12 @@
     <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>33</v>
+      </c>
+      <c r="B29" s="9">
+        <v>45287</v>
+      </c>
+      <c r="C29" s="9">
+        <v>45287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show payroll history No payroll exists message Invalid employee id message Save success message relisting after save implement clear
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t xml:space="preserve">Show payroll history </t>
+  </si>
+  <si>
+    <t xml:space="preserve">relisting after save </t>
+  </si>
+  <si>
+    <t>implement clear</t>
   </si>
 </sst>
 </file>
@@ -658,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B36" sqref="B36:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -997,25 +1003,77 @@
       <c r="A30" t="s">
         <v>82</v>
       </c>
+      <c r="B30" s="9">
+        <v>45289</v>
+      </c>
+      <c r="C30" s="9">
+        <v>45289</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>86</v>
       </c>
+      <c r="B31" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C31" s="9">
+        <v>45290</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C32" s="9">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C33" s="9">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>85</v>
+      </c>
+      <c r="B34" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C34" s="9">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="9">
+        <v>45290</v>
+      </c>
+      <c r="C36" s="9">
+        <v>45290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Usability Fixes and Generate Salary Partial
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -15,7 +15,6 @@
     <sheet name="create employee screen" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1472,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P13" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29:AO29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Disable auto complete , Payroll doesnt exist message , Log write to file
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5595" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5595"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="Generate Salary screen" sheetId="6" r:id="rId2"/>
-    <sheet name="View Salary screen " sheetId="5" r:id="rId3"/>
-    <sheet name="Bugs" sheetId="2" r:id="rId4"/>
+    <sheet name="Bugs" sheetId="2" r:id="rId2"/>
+    <sheet name="Generate Salary screen" sheetId="6" r:id="rId3"/>
+    <sheet name="View Salary screen " sheetId="5" r:id="rId4"/>
     <sheet name="Test data backup" sheetId="4" r:id="rId5"/>
     <sheet name="create employee screen" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -512,6 +512,36 @@
   </si>
   <si>
     <t>List button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end to end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log Writing to File </t>
+  </si>
+  <si>
+    <t>Converting to a desktop app using enzyme</t>
+  </si>
+  <si>
+    <t>Encryption of sensitive data in .env files</t>
+  </si>
+  <si>
+    <t>Salary Screen</t>
+  </si>
+  <si>
+    <t>open bugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doubt : where is leaves availed used </t>
+  </si>
+  <si>
+    <t xml:space="preserve">once Alert Panel is dismissed not able to render new alerts </t>
+  </si>
+  <si>
+    <t>No message shown when payroll is not saved..instead shows a stack trac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable auto complete </t>
   </si>
 </sst>
 </file>
@@ -963,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1331,7 +1361,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -1342,7 +1372,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -1353,7 +1383,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -1364,7 +1394,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1386,7 +1416,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1397,7 +1427,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1408,7 +1438,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -1419,12 +1449,12 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>158</v>
       </c>
@@ -1435,7 +1465,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>157</v>
       </c>
@@ -1446,7 +1476,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>159</v>
       </c>
@@ -1457,9 +1487,140 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>160</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44927</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="1">
+        <v>44940</v>
+      </c>
+      <c r="C48" s="1">
+        <v>44940</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44940</v>
+      </c>
+      <c r="C50" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" s="1">
+        <v>44940</v>
+      </c>
+      <c r="C55" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1467,11 +1628,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
@@ -1933,7 +2094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1985,53 +2146,6 @@
     <row r="9" spans="1:2">
       <c r="B9" t="s">
         <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Process Company Salary and its Status
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -9,10 +9,10 @@
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
-    <sheet name="Generate Salary screen" sheetId="6" r:id="rId3"/>
-    <sheet name="View Salary screen " sheetId="5" r:id="rId4"/>
-    <sheet name="Test data backup" sheetId="4" r:id="rId5"/>
-    <sheet name="create employee screen" sheetId="3" r:id="rId6"/>
+    <sheet name="Test data backup" sheetId="4" r:id="rId3"/>
+    <sheet name="create employee screen" sheetId="3" r:id="rId4"/>
+    <sheet name="Generate Salary screen" sheetId="6" r:id="rId5"/>
+    <sheet name="View Salary screen " sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="179">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -542,6 +542,27 @@
   </si>
   <si>
     <t xml:space="preserve">Disable auto complete </t>
+  </si>
+  <si>
+    <t>Fix style issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make a demo </t>
+  </si>
+  <si>
+    <t>Top Navigation Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation from Employee Details to Payroll and Salary Screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Generation </t>
+  </si>
+  <si>
+    <t>clarification raised</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
 </sst>
 </file>
@@ -993,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="A52" sqref="A52:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1512,9 +1533,20 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44940</v>
+      </c>
+      <c r="C49" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B50" s="1">
         <v>44940</v>
@@ -1523,35 +1555,58 @@
         <v>44940</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44940</v>
+      </c>
+      <c r="C51" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>171</v>
-      </c>
-      <c r="B55" s="1">
-        <v>44940</v>
-      </c>
-      <c r="C55" s="1">
-        <v>44940</v>
       </c>
     </row>
   </sheetData>
@@ -1565,7 +1620,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,6 +1661,9 @@
       <c r="A5" t="s">
         <v>169</v>
       </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
@@ -1630,9 +1688,207 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>9447757072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="24">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="36">
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="36">
+      <c r="K7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="36">
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="36">
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="36">
+      <c r="B16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="36">
+      <c r="B18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="36">
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="36">
+      <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
@@ -2094,7 +2350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2151,202 +2407,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>9447757072</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="24">
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="36">
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="36">
-      <c r="K7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="36">
-      <c r="B11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="36">
-      <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="36">
-      <c r="B16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="36">
-      <c r="B18" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="36">
-      <c r="B20" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="36">
-      <c r="B22" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Style Issues , Menu Bar
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:D59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1583,6 +1583,12 @@
       <c r="A54" t="s">
         <v>172</v>
       </c>
+      <c r="B54" s="1">
+        <v>44941</v>
+      </c>
+      <c r="C54" s="1">
+        <v>44941</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
@@ -1592,6 +1598,12 @@
     <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>174</v>
+      </c>
+      <c r="B56" s="1">
+        <v>44941</v>
+      </c>
+      <c r="C56" s="1">
+        <v>44941</v>
       </c>
     </row>
     <row r="57" spans="1:4">

</xml_diff>

<commit_message>
Salary Generate Bugs , Process Salary Screen
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="200">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -547,9 +547,6 @@
     <t>Fix style issues</t>
   </si>
   <si>
-    <t xml:space="preserve">Make a demo </t>
-  </si>
-  <si>
     <t>Top Navigation Menu</t>
   </si>
   <si>
@@ -595,19 +592,40 @@
     <t>client side only</t>
   </si>
   <si>
-    <t>server side only</t>
-  </si>
-  <si>
-    <t>code clean up at server side only</t>
-  </si>
-  <si>
     <t>Export feature</t>
   </si>
   <si>
-    <t xml:space="preserve">both client and server new field in api response also change the message displayed on save button click </t>
-  </si>
-  <si>
-    <t xml:space="preserve">client side and server side change existing finalize api also display the message on finalize button click </t>
+    <t xml:space="preserve">Generate Salary Bugs </t>
+  </si>
+  <si>
+    <t>Clicked on clear employee code is not clearred</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Change the text "Enter the input fields to calculate salary"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premature button errors </t>
+  </si>
+  <si>
+    <t>Salary is finalized still I am able to click on save…</t>
+  </si>
+  <si>
+    <t>Date of Payment is not being checked</t>
+  </si>
+  <si>
+    <t>Salary finalize message is not correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make a new demo </t>
+  </si>
+  <si>
+    <t>Final Usability Enhancements</t>
+  </si>
+  <si>
+    <t>Non Functional Requirements</t>
   </si>
 </sst>
 </file>
@@ -656,7 +674,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,6 +684,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,6 +803,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1615,13 +1640,24 @@
       <c r="A52" t="s">
         <v>168</v>
       </c>
-      <c r="D52" t="s">
-        <v>176</v>
+      <c r="D52" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44941</v>
+      </c>
+      <c r="C53" s="1">
+        <v>44941</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" s="1">
         <v>44941</v>
@@ -1631,110 +1667,130 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>173</v>
+      <c r="A55" s="17" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>174</v>
-      </c>
-      <c r="B56" s="1">
-        <v>44941</v>
-      </c>
-      <c r="C56" s="1">
-        <v>44941</v>
+      <c r="A56" s="17" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>179</v>
+      </c>
+      <c r="B57" s="1">
+        <v>44942</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44945</v>
+      </c>
+      <c r="D57" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>180</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44942</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44945</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>186</v>
+      </c>
+      <c r="D59" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="17" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="17" t="s">
-        <v>178</v>
+      <c r="A61" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44945</v>
+      </c>
+      <c r="C61" s="1">
+        <v>44945</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="17" t="s">
-        <v>179</v>
+      <c r="A62" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44945</v>
+      </c>
+      <c r="C62" s="1">
+        <v>44945</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D63" t="s">
-        <v>192</v>
+        <v>185</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44945</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44945</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>181</v>
-      </c>
-      <c r="D64" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>184</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44945</v>
+      </c>
+      <c r="C64" s="1">
+        <v>44945</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>184</v>
-      </c>
-      <c r="D68" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>186</v>
-      </c>
-      <c r="D69" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>185</v>
-      </c>
-      <c r="D70" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1745,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1786,11 +1842,11 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1807,6 +1863,59 @@
       </c>
       <c r="B7" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINAL save Bug fixed
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -756,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -804,6 +804,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -1687,7 +1688,7 @@
         <v>44945</v>
       </c>
       <c r="D57" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1804,7 +1805,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1911,11 +1912,11 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>196</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alert Panel Dismiss Bug Fixed
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FE7EDD-8B0F-435E-8A2B-F5C9DB27F56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F05C97-B61B-4F3F-B00D-EBCFB05C14F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="230">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -556,9 +556,6 @@
   </si>
   <si>
     <t>clarification raised</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t xml:space="preserve">Changes to salary finalize </t>
@@ -769,7 +766,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,12 +776,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,13 +900,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
@@ -1780,17 +1771,17 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B57" s="1">
         <v>44942</v>
@@ -1804,7 +1795,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B58" s="1">
         <v>44942</v>
@@ -1815,7 +1806,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B59" s="1">
         <v>44945</v>
@@ -1826,12 +1817,12 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B61" s="1">
         <v>44945</v>
@@ -1842,7 +1833,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B62" s="1">
         <v>44945</v>
@@ -1853,7 +1844,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B63" s="1">
         <v>44945</v>
@@ -1864,7 +1855,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B64" s="1">
         <v>44945</v>
@@ -1875,7 +1866,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B65" s="1">
         <v>45317</v>
@@ -1886,12 +1877,12 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1901,7 +1892,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1916,7 +1907,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B75" s="1">
         <v>45316</v>
@@ -1927,7 +1918,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B76" s="1">
         <v>45316</v>
@@ -1938,7 +1929,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B77" s="1">
         <v>45316</v>
@@ -1949,7 +1940,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B79" s="1">
         <v>45324</v>
@@ -1960,7 +1951,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B80" s="1">
         <v>45324</v>
@@ -1971,7 +1962,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B81" s="1">
         <v>45324</v>
@@ -1982,7 +1973,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B82" s="1">
         <v>45321</v>
@@ -1993,7 +1984,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2006,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2045,11 +2036,11 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2070,55 +2061,55 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
         <v>189</v>
-      </c>
-      <c r="B11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2807,13 +2798,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>203</v>
-      </c>
-      <c r="E1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24">
@@ -2829,8 +2820,8 @@
       <c r="F2" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>205</v>
+      <c r="G2" s="18" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2847,7 +2838,7 @@
         <v>116</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36">
@@ -2861,7 +2852,7 @@
         <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24">
@@ -2877,8 +2868,8 @@
       <c r="F5" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>208</v>
+      <c r="G5" s="18" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60">
@@ -2892,7 +2883,7 @@
         <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="48">
@@ -2906,7 +2897,7 @@
         <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24">
@@ -2917,7 +2908,7 @@
         <v>123</v>
       </c>
       <c r="G8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24">
@@ -2925,7 +2916,7 @@
         <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="48">
@@ -2933,7 +2924,7 @@
         <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24">
@@ -2941,7 +2932,7 @@
         <v>126</v>
       </c>
       <c r="G11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="36">
@@ -2954,12 +2945,12 @@
         <v>129</v>
       </c>
       <c r="G13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24">
+      <c r="E15" s="19" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="24">
-      <c r="E15" s="20" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="17" spans="5:7" ht="48">
@@ -2967,7 +2958,7 @@
         <v>130</v>
       </c>
       <c r="G17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="5:7" ht="36">
@@ -2975,7 +2966,7 @@
         <v>131</v>
       </c>
       <c r="G18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="5:7">
@@ -2983,7 +2974,7 @@
         <v>132</v>
       </c>
       <c r="G19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="5:7" ht="24">
@@ -2991,7 +2982,7 @@
         <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="5:7" ht="24">
@@ -2999,7 +2990,7 @@
         <v>134</v>
       </c>
       <c r="G21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="5:7" ht="24">
@@ -3007,7 +2998,7 @@
         <v>135</v>
       </c>
       <c r="G22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="5:7" ht="48">
@@ -3015,7 +3006,7 @@
         <v>136</v>
       </c>
       <c r="G23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="5:7" ht="24">
@@ -3023,7 +3014,7 @@
         <v>137</v>
       </c>
       <c r="G24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="5:7" ht="24">
@@ -3031,7 +3022,7 @@
         <v>138</v>
       </c>
       <c r="G25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="5:7" ht="36">

</xml_diff>

<commit_message>
In process salary screen not able to change filter criteria and list
</commit_message>
<xml_diff>
--- a/Work_Progress.xlsx
+++ b/Work_Progress.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F05C97-B61B-4F3F-B00D-EBCFB05C14F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B58E8C7-B4C9-4A67-9920-673B46FFB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="New Gen Salary Screen" sheetId="7" r:id="rId6"/>
     <sheet name="View Salary screen " sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="237">
   <si>
     <t xml:space="preserve">Use Mongoose framework to create EmployeeSchema </t>
   </si>
@@ -718,6 +729,27 @@
   </si>
   <si>
     <t>Cosmetic issues in report</t>
+  </si>
+  <si>
+    <t>Cosmetic Issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In process salary screen not able to change filter criteria and list </t>
+  </si>
+  <si>
+    <t>Missing Total</t>
+  </si>
+  <si>
+    <t>Missing Sl No</t>
+  </si>
+  <si>
+    <t>title should be in bold and size should be large and rowspan should be 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column header should be in bold and row span should be 3 </t>
+  </si>
+  <si>
+    <t>need to increase column width of all columns 25 px</t>
   </si>
 </sst>
 </file>
@@ -853,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,7 +938,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2036,7 +2067,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" t="s">
         <v>169</v>
       </c>
       <c r="B5" t="s">
@@ -2110,6 +2141,44 @@
       </c>
       <c r="B16" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>